<commit_message>
Update functional requirement v1.1
</commit_message>
<xml_diff>
--- a/tmp/Requirements.xlsx
+++ b/tmp/Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoang\OneDrive\Máy tính\SEFinalProject\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577C6D85-87AD-4DCC-A0BB-80F345C2FFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33189419-D67E-4CCB-9C67-A89AB974940A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -49,33 +49,12 @@
     <t>Order management</t>
   </si>
   <si>
-    <t>Want</t>
-  </si>
-  <si>
-    <t>Sales tracking</t>
-  </si>
-  <si>
-    <t>Payment processing</t>
-  </si>
-  <si>
     <t>Inventory management</t>
   </si>
   <si>
-    <t>Reporting and Analytics</t>
-  </si>
-  <si>
-    <t>User management</t>
-  </si>
-  <si>
     <t>Product Management</t>
   </si>
   <si>
-    <t>Accountants shall be able to process orders, tracking orders status, generate invoices,…</t>
-  </si>
-  <si>
-    <t>Resellers shall be able to place an order of items and choose a payment method. They also make an online payment and see the status of their orders.</t>
-  </si>
-  <si>
     <t>FR-01</t>
   </si>
   <si>
@@ -106,9 +85,6 @@
     <t>FR-10</t>
   </si>
   <si>
-    <t>Customers shall be able to manage customer profiles, place orders, choose payment method</t>
-  </si>
-  <si>
     <t>FR-11</t>
   </si>
   <si>
@@ -121,31 +97,52 @@
     <t>Accountants shall be able to add, delete, edit product information.</t>
   </si>
   <si>
-    <t>This system should be able to track sales, generate reports on sales, …</t>
-  </si>
-  <si>
-    <t>Customers, resellers should be able to process payments, generate receipts, …</t>
-  </si>
-  <si>
     <t>Operators shall be able to manage user profiles and accounts, assign user roles and permissions, control access to sensitive data, generating reports on users, …</t>
   </si>
   <si>
-    <t>Accountants should be able to track sales, view incoming/outgoing stock reports, generate reports on sales, …</t>
-  </si>
-  <si>
-    <t>Accountants shall be able to create goods received when the distributor imports goods.</t>
-  </si>
-  <si>
-    <t>Delivery management</t>
-  </si>
-  <si>
-    <t>Accountants shall be able to create goods delivery note to deliver goods to resellers, update the status of orders as being transferred and update the payment status of resellers</t>
-  </si>
-  <si>
-    <t>Customer service provider</t>
-  </si>
-  <si>
-    <t>Reseller service provider</t>
+    <t xml:space="preserve">Accountants shall be able to  manage inventory by creating a Goods Received Note when goods are imported into the warehouse. </t>
+  </si>
+  <si>
+    <t>Payment Integration</t>
+  </si>
+  <si>
+    <t>Order Placement</t>
+  </si>
+  <si>
+    <t>Resellers/customers should be able to place an order for items by selecting the desired products, specifying the quantity, and choosing a payment method (Cash, bank transfer, Momo...).</t>
+  </si>
+  <si>
+    <t>Order Status Tracking</t>
+  </si>
+  <si>
+    <t>Resellers/customers should be able to track the status of their orders, including knowing when the order has been processed, shipped, or delivered.</t>
+  </si>
+  <si>
+    <t>Accountants shall be able to create goods delivery note to deliver goods to resellers, update the status of orders as being transferred.</t>
+  </si>
+  <si>
+    <t>Accountants shall be able to process orders, track and update orders and payments status, generate invoices.  Resellers/customers should also be able to view the payment status of their orders.</t>
+  </si>
+  <si>
+    <t>The software should be integrated with different payment gateways, allowing resellers/customers to make online payments through the platform.</t>
+  </si>
+  <si>
+    <t>Delivery Management</t>
+  </si>
+  <si>
+    <t>User Management</t>
+  </si>
+  <si>
+    <t>Stock Reporting</t>
+  </si>
+  <si>
+    <t>The software should provide incoming/outgoing stock reports, allowing accountants to view stock levels, track inventory movements, and manage stock levels efficiently.</t>
+  </si>
+  <si>
+    <t>Sales Reporting</t>
+  </si>
+  <si>
+    <t>The software should provide sales reporting and revenue reports, allowing accountants to view best-selling products, track sales trends, and forecast sales performance.</t>
   </si>
 </sst>
 </file>
@@ -204,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
@@ -215,19 +212,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -236,6 +230,10 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
@@ -248,19 +246,15 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
@@ -292,23 +286,23 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DA53702-2EBA-4F3F-88E3-C43D885C245F}" name="Table1" displayName="Table1" ref="B4:E17" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="B4:E17" xr:uid="{3DA53702-2EBA-4F3F-88E3-C43D885C245F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FE2820DE-CCA8-4474-A32C-D871001B9929}" name="ID" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{DE861C93-FDCA-4761-A323-7789CA10AA36}" name="Functional requirements" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{70561D6F-F0AF-40B6-AC7F-F64DE5E23767}" name="Must / Want" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{80625612-35E0-4B72-B73D-A4B365705E34}" name="Description" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{FE2820DE-CCA8-4474-A32C-D871001B9929}" name="ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{DE861C93-FDCA-4761-A323-7789CA10AA36}" name="Functional requirements" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{70561D6F-F0AF-40B6-AC7F-F64DE5E23767}" name="Must / Want" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{80625612-35E0-4B72-B73D-A4B365705E34}" name="Description" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{44AB80CB-75B9-4CF2-A4D5-0B3B63BB3FB0}" name="Table13" displayName="Table13" ref="B4:E11" totalsRowShown="0" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{44AB80CB-75B9-4CF2-A4D5-0B3B63BB3FB0}" name="Table13" displayName="Table13" ref="B4:E11" totalsRowShown="0" dataDxfId="4">
   <autoFilter ref="B4:E11" xr:uid="{44AB80CB-75B9-4CF2-A4D5-0B3B63BB3FB0}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9DC6B6F2-95B1-43EB-9EF3-0913D398AD36}" name="ID" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{41A6AE69-FD09-4606-918B-EA7AD346CEBA}" name="Non-Functional requirements" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{FC0CD7AA-76B8-4E3F-9616-F36481092CEA}" name="Must / Want" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{C9EDB3C6-6DB6-4CAE-99CB-282E208B6620}" name="Description" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{9DC6B6F2-95B1-43EB-9EF3-0913D398AD36}" name="ID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{41A6AE69-FD09-4606-918B-EA7AD346CEBA}" name="Non-Functional requirements" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{FC0CD7AA-76B8-4E3F-9616-F36481092CEA}" name="Must / Want" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{C9EDB3C6-6DB6-4CAE-99CB-282E208B6620}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -579,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,23 +601,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -632,124 +626,124 @@
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
@@ -757,7 +751,7 @@
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
@@ -765,7 +759,7 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="3"/>

</xml_diff>

<commit_message>
Structure change - add usecase diagrams
</commit_message>
<xml_diff>
--- a/tmp/Requirements.xlsx
+++ b/tmp/Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoang\OneDrive\Máy tính\SEFinalProject\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33189419-D67E-4CCB-9C67-A89AB974940A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD58295C-3F87-4604-AE5D-17D35D5D3DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -97,15 +97,6 @@
     <t>Accountants shall be able to add, delete, edit product information.</t>
   </si>
   <si>
-    <t>Operators shall be able to manage user profiles and accounts, assign user roles and permissions, control access to sensitive data, generating reports on users, …</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accountants shall be able to  manage inventory by creating a Goods Received Note when goods are imported into the warehouse. </t>
-  </si>
-  <si>
-    <t>Payment Integration</t>
-  </si>
-  <si>
     <t>Order Placement</t>
   </si>
   <si>
@@ -115,18 +106,12 @@
     <t>Order Status Tracking</t>
   </si>
   <si>
-    <t>Resellers/customers should be able to track the status of their orders, including knowing when the order has been processed, shipped, or delivered.</t>
-  </si>
-  <si>
     <t>Accountants shall be able to create goods delivery note to deliver goods to resellers, update the status of orders as being transferred.</t>
   </si>
   <si>
     <t>Accountants shall be able to process orders, track and update orders and payments status, generate invoices.  Resellers/customers should also be able to view the payment status of their orders.</t>
   </si>
   <si>
-    <t>The software should be integrated with different payment gateways, allowing resellers/customers to make online payments through the platform.</t>
-  </si>
-  <si>
     <t>Delivery Management</t>
   </si>
   <si>
@@ -143,6 +128,15 @@
   </si>
   <si>
     <t>The software should provide sales reporting and revenue reports, allowing accountants to view best-selling products, track sales trends, and forecast sales performance.</t>
+  </si>
+  <si>
+    <t>Accountants shall be able to  manage inventory by creating a Goods Received/Delivery Note, when goods are imported into the warehouse or exported to resellers.</t>
+  </si>
+  <si>
+    <t>Resellers/customers and accountants should be able to track the status of their orders, including knowing when the order has been processed, shipped, or delivered.</t>
+  </si>
+  <si>
+    <t>Admin shall be able to manage user profiles and accounts, assign user roles and permissions, control access to sensitive data, generating reports on users, …</t>
   </si>
 </sst>
 </file>
@@ -574,7 +568,7 @@
   <dimension ref="B4:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +595,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
@@ -612,7 +606,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="60" x14ac:dyDescent="0.25">
@@ -626,7 +620,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="60" x14ac:dyDescent="0.25">
@@ -634,27 +628,27 @@
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="60" x14ac:dyDescent="0.25">
@@ -662,13 +656,13 @@
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -690,41 +684,35 @@
         <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="60" x14ac:dyDescent="0.25">
@@ -732,13 +720,13 @@
         <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>